<commit_message>
deactivate IT Tech Support Specialist page
</commit_message>
<xml_diff>
--- a/static/programlisting.xlsx
+++ b/static/programlisting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\aolccbc.com\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC286B99-15C0-4BB2-A419-3D63206A7F7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951F34EC-5026-4301-AB7E-223E05C5AFB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2353,8 +2353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4946,7 +4946,7 @@
         <v>20000</v>
       </c>
       <c r="H52" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="I52" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Correct pricing on a couple of programs
</commit_message>
<xml_diff>
--- a/static/programlisting.xlsx
+++ b/static/programlisting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\aolccbc.com\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951F34EC-5026-4301-AB7E-223E05C5AFB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7369565-763D-4404-AF60-CF2F6704B3B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -722,59 +722,59 @@
       <sheetName val="Reference"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
       <sheetData sheetId="53">
         <row r="5">
           <cell r="A5" t="str">
@@ -872,7 +872,7 @@
             <v>141</v>
           </cell>
           <cell r="H13">
-            <v>657</v>
+            <v>22293</v>
           </cell>
         </row>
         <row r="14">
@@ -883,7 +883,7 @@
             <v>136</v>
           </cell>
           <cell r="H14">
-            <v>499</v>
+            <v>17893</v>
           </cell>
         </row>
         <row r="15">
@@ -2047,8 +2047,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2354,7 +2354,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,11 +2419,11 @@
         <v>A+ Network+ And Mcsa Desktop Cert. Prep</v>
       </c>
       <c r="B2" s="1">
-        <f t="shared" ref="B2:B33" si="0">C2/weeks</f>
+        <f t="shared" ref="B2:B33" ca="1" si="0">C2/weeks</f>
         <v>34.090909090909093</v>
       </c>
       <c r="C2" s="1">
-        <f>[1]Summary!$G5</f>
+        <f ca="1">[1]Summary!$G5</f>
         <v>750</v>
       </c>
       <c r="D2" t="s">
@@ -2437,7 +2437,7 @@
         <v>Certificate</v>
       </c>
       <c r="G2">
-        <f>[1]Summary!$H5</f>
+        <f ca="1">[1]Summary!$H5</f>
         <v>8510</v>
       </c>
       <c r="H2" t="s">
@@ -2469,11 +2469,11 @@
         <v>Accounting Administrator Diploma With Sage</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>35.863636363636367</v>
       </c>
       <c r="C3" s="1">
-        <f>[1]Summary!$G6</f>
+        <f ca="1">[1]Summary!$G6</f>
         <v>789</v>
       </c>
       <c r="D3" t="s">
@@ -2487,7 +2487,7 @@
         <v>Diploma</v>
       </c>
       <c r="G3">
-        <f>[1]Summary!$H6</f>
+        <f ca="1">[1]Summary!$H6</f>
         <v>11559</v>
       </c>
       <c r="H3" t="s">
@@ -2519,11 +2519,11 @@
         <v>Accounting And Business Technology Diploma</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>40.863636363636367</v>
       </c>
       <c r="C4" s="1">
-        <f>[1]Summary!$G7</f>
+        <f ca="1">[1]Summary!$G7</f>
         <v>899</v>
       </c>
       <c r="D4" t="s">
@@ -2537,7 +2537,7 @@
         <v>Diploma</v>
       </c>
       <c r="G4">
-        <f>[1]Summary!$H7</f>
+        <f ca="1">[1]Summary!$H7</f>
         <v>12729</v>
       </c>
       <c r="H4" t="s">
@@ -2569,11 +2569,11 @@
         <v>Accounting And Payroll Administrator Diploma</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>49.272727272727273</v>
       </c>
       <c r="C5" s="1">
-        <f>[1]Summary!$G8</f>
+        <f ca="1">[1]Summary!$G8</f>
         <v>1084</v>
       </c>
       <c r="D5" t="s">
@@ -2587,7 +2587,7 @@
         <v>Diploma</v>
       </c>
       <c r="G5">
-        <f>[1]Summary!$H8</f>
+        <f ca="1">[1]Summary!$H8</f>
         <v>15180</v>
       </c>
       <c r="H5" t="s">
@@ -2619,11 +2619,11 @@
         <v>Accounting Bookkeeper Certificate</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>29.227272727272727</v>
       </c>
       <c r="C6" s="1">
-        <f>[1]Summary!$G9</f>
+        <f ca="1">[1]Summary!$G9</f>
         <v>643</v>
       </c>
       <c r="D6" t="s">
@@ -2637,7 +2637,7 @@
         <v>Certificate</v>
       </c>
       <c r="G6">
-        <f>[1]Summary!$H9</f>
+        <f ca="1">[1]Summary!$H9</f>
         <v>8707</v>
       </c>
       <c r="H6" t="s">
@@ -2669,11 +2669,11 @@
         <v>Accounting Clerk Certificate</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>20.90909090909091</v>
       </c>
       <c r="C7" s="1">
-        <f>[1]Summary!$G10</f>
+        <f ca="1">[1]Summary!$G10</f>
         <v>460</v>
       </c>
       <c r="D7" t="s">
@@ -2687,7 +2687,7 @@
         <v>Certificate</v>
       </c>
       <c r="G7">
-        <f>[1]Summary!$H10</f>
+        <f ca="1">[1]Summary!$H10</f>
         <v>6452</v>
       </c>
       <c r="H7" t="s">
@@ -2719,11 +2719,11 @@
         <v>Addictions Worker Certificate</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>13.636363636363637</v>
       </c>
       <c r="C8" s="1">
-        <f>[1]Summary!$G11</f>
+        <f ca="1">[1]Summary!$G11</f>
         <v>300</v>
       </c>
       <c r="D8" t="s">
@@ -2737,7 +2737,7 @@
         <v>Certificate</v>
       </c>
       <c r="G8">
-        <f>[1]Summary!$H11</f>
+        <f ca="1">[1]Summary!$H11</f>
         <v>3079</v>
       </c>
       <c r="H8" t="s">
@@ -2769,11 +2769,11 @@
         <v>Administrative Assistant Diploma</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>34.909090909090907</v>
       </c>
       <c r="C9" s="1">
-        <f>[1]Summary!$G12</f>
+        <f ca="1">[1]Summary!$G12</f>
         <v>768</v>
       </c>
       <c r="D9" t="s">
@@ -2787,7 +2787,7 @@
         <v>Diploma</v>
       </c>
       <c r="G9">
-        <f>[1]Summary!$H12</f>
+        <f ca="1">[1]Summary!$H12</f>
         <v>10097</v>
       </c>
       <c r="H9" t="s">
@@ -2819,11 +2819,11 @@
         <v>Business Administration Co-Op Diploma</v>
       </c>
       <c r="B10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>6.4090909090909092</v>
       </c>
       <c r="C10" s="1">
-        <f>[1]Summary!$G13</f>
+        <f ca="1">[1]Summary!$G13</f>
         <v>141</v>
       </c>
       <c r="D10" t="s">
@@ -2837,8 +2837,8 @@
         <v>Diploma</v>
       </c>
       <c r="G10">
-        <f>[1]Summary!$H13</f>
-        <v>657</v>
+        <f ca="1">[1]Summary!$H13</f>
+        <v>22293</v>
       </c>
       <c r="H10" t="s">
         <v>13</v>
@@ -2869,11 +2869,11 @@
         <v>Business Administration Diploma</v>
       </c>
       <c r="B11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>6.1818181818181817</v>
       </c>
       <c r="C11" s="1">
-        <f>[1]Summary!$G14</f>
+        <f ca="1">[1]Summary!$G14</f>
         <v>136</v>
       </c>
       <c r="D11" t="s">
@@ -2887,8 +2887,8 @@
         <v>Diploma</v>
       </c>
       <c r="G11">
-        <f>[1]Summary!$H14</f>
-        <v>499</v>
+        <f ca="1">[1]Summary!$H14</f>
+        <v>17893</v>
       </c>
       <c r="H11" t="s">
         <v>13</v>
@@ -2919,11 +2919,11 @@
         <v>Business Management Certificate</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>28.045454545454547</v>
       </c>
       <c r="C12" s="1">
-        <f>[1]Summary!$G15</f>
+        <f ca="1">[1]Summary!$G15</f>
         <v>617</v>
       </c>
       <c r="D12" t="s">
@@ -2937,7 +2937,7 @@
         <v>Certificate</v>
       </c>
       <c r="G12">
-        <f>[1]Summary!$H15</f>
+        <f ca="1">[1]Summary!$H15</f>
         <v>9329</v>
       </c>
       <c r="H12" t="s">
@@ -2969,11 +2969,11 @@
         <v>Business Office Skills Diploma</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>38.31818181818182</v>
       </c>
       <c r="C13" s="1">
-        <f>[1]Summary!$G16</f>
+        <f ca="1">[1]Summary!$G16</f>
         <v>843</v>
       </c>
       <c r="D13" t="s">
@@ -2987,7 +2987,7 @@
         <v>Diploma</v>
       </c>
       <c r="G13">
-        <f>[1]Summary!$H16</f>
+        <f ca="1">[1]Summary!$H16</f>
         <v>11409</v>
       </c>
       <c r="H13" t="s">
@@ -3019,11 +3019,11 @@
         <v>Business Receptionist Certificate</v>
       </c>
       <c r="B14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>24.59090909090909</v>
       </c>
       <c r="C14" s="1">
-        <f>[1]Summary!$G17</f>
+        <f ca="1">[1]Summary!$G17</f>
         <v>541</v>
       </c>
       <c r="D14" t="s">
@@ -3037,7 +3037,7 @@
         <v>Certificate</v>
       </c>
       <c r="G14">
-        <f>[1]Summary!$H17</f>
+        <f ca="1">[1]Summary!$H17</f>
         <v>7135</v>
       </c>
       <c r="H14" t="s">
@@ -3069,11 +3069,11 @@
         <v>Business Service Essentials Co-Op Diploma</v>
       </c>
       <c r="B15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>48.909090909090907</v>
       </c>
       <c r="C15" s="1">
-        <f>[1]Summary!$G18</f>
+        <f ca="1">[1]Summary!$G18</f>
         <v>1076</v>
       </c>
       <c r="D15" t="s">
@@ -3087,7 +3087,7 @@
         <v>Diploma</v>
       </c>
       <c r="G15">
-        <f>[1]Summary!$H18</f>
+        <f ca="1">[1]Summary!$H18</f>
         <v>10752</v>
       </c>
       <c r="H15" t="s">
@@ -3119,11 +3119,11 @@
         <v>Call Centre Customer Representative Diploma</v>
       </c>
       <c r="B16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>31.181818181818183</v>
       </c>
       <c r="C16" s="1">
-        <f>[1]Summary!$G19</f>
+        <f ca="1">[1]Summary!$G19</f>
         <v>686</v>
       </c>
       <c r="D16" t="s">
@@ -3137,7 +3137,7 @@
         <v>Diploma</v>
       </c>
       <c r="G16">
-        <f>[1]Summary!$H19</f>
+        <f ca="1">[1]Summary!$H19</f>
         <v>9627</v>
       </c>
       <c r="H16" t="s">
@@ -3169,11 +3169,11 @@
         <v>Community Service Worker And Addictions Worker Diploma</v>
       </c>
       <c r="B17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>52.590909090909093</v>
       </c>
       <c r="C17" s="1">
-        <f>[1]Summary!$G20</f>
+        <f ca="1">[1]Summary!$G20</f>
         <v>1157</v>
       </c>
       <c r="D17" t="s">
@@ -3187,7 +3187,7 @@
         <v>Diploma</v>
       </c>
       <c r="G17">
-        <f>[1]Summary!$H20</f>
+        <f ca="1">[1]Summary!$H20</f>
         <v>15449</v>
       </c>
       <c r="H17" t="s">
@@ -3219,11 +3219,11 @@
         <v>Community Service Worker Diploma</v>
       </c>
       <c r="B18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>37.590909090909093</v>
       </c>
       <c r="C18" s="1">
-        <f>[1]Summary!$G21</f>
+        <f ca="1">[1]Summary!$G21</f>
         <v>827</v>
       </c>
       <c r="D18" t="s">
@@ -3237,7 +3237,7 @@
         <v>Diploma</v>
       </c>
       <c r="G18">
-        <f>[1]Summary!$H21</f>
+        <f ca="1">[1]Summary!$H21</f>
         <v>12370</v>
       </c>
       <c r="H18" t="s">
@@ -3272,11 +3272,11 @@
         <v>Computer Service Technician Certificate</v>
       </c>
       <c r="B19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>26.636363636363637</v>
       </c>
       <c r="C19" s="1">
-        <f>[1]Summary!$G22</f>
+        <f ca="1">[1]Summary!$G22</f>
         <v>586</v>
       </c>
       <c r="D19" t="s">
@@ -3290,7 +3290,7 @@
         <v>Certificate</v>
       </c>
       <c r="G19">
-        <f>[1]Summary!$H22</f>
+        <f ca="1">[1]Summary!$H22</f>
         <v>5822</v>
       </c>
       <c r="H19" t="s">
@@ -3325,11 +3325,11 @@
         <v>Computer Service Technician Diploma</v>
       </c>
       <c r="B20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>46.31818181818182</v>
       </c>
       <c r="C20" s="1">
-        <f>[1]Summary!$G23</f>
+        <f ca="1">[1]Summary!$G23</f>
         <v>1019</v>
       </c>
       <c r="D20" t="s">
@@ -3343,7 +3343,7 @@
         <v>Diploma</v>
       </c>
       <c r="G20">
-        <f>[1]Summary!$H23</f>
+        <f ca="1">[1]Summary!$H23</f>
         <v>12167</v>
       </c>
       <c r="H20" t="s">
@@ -3378,11 +3378,11 @@
         <v>Computer Software Support Diploma</v>
       </c>
       <c r="B21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>46.31818181818182</v>
       </c>
       <c r="C21" s="1">
-        <f>[1]Summary!$G24</f>
+        <f ca="1">[1]Summary!$G24</f>
         <v>1019</v>
       </c>
       <c r="D21" t="s">
@@ -3396,7 +3396,7 @@
         <v>Diploma</v>
       </c>
       <c r="G21">
-        <f>[1]Summary!$H24</f>
+        <f ca="1">[1]Summary!$H24</f>
         <v>12167</v>
       </c>
       <c r="H21" t="s">
@@ -3428,11 +3428,11 @@
         <v>Computerized Office Procedures Certificate</v>
       </c>
       <c r="B22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>25.59090909090909</v>
       </c>
       <c r="C22" s="1">
-        <f>[1]Summary!$G25</f>
+        <f ca="1">[1]Summary!$G25</f>
         <v>563</v>
       </c>
       <c r="D22" t="s">
@@ -3446,7 +3446,7 @@
         <v>Certificate</v>
       </c>
       <c r="G22">
-        <f>[1]Summary!$H25</f>
+        <f ca="1">[1]Summary!$H25</f>
         <v>7132</v>
       </c>
       <c r="H22" t="s">
@@ -3478,11 +3478,11 @@
         <v>Conference And Event Planner Diploma</v>
       </c>
       <c r="B23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>46.227272727272727</v>
       </c>
       <c r="C23" s="1">
-        <f>[1]Summary!$G26</f>
+        <f ca="1">[1]Summary!$G26</f>
         <v>1017</v>
       </c>
       <c r="D23" t="s">
@@ -3496,7 +3496,7 @@
         <v>Diploma</v>
       </c>
       <c r="G23">
-        <f>[1]Summary!$H26</f>
+        <f ca="1">[1]Summary!$H26</f>
         <v>14474</v>
       </c>
       <c r="H23" t="s">
@@ -3528,11 +3528,11 @@
         <v>Customer Service Representative Certificate</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>20.727272727272727</v>
       </c>
       <c r="C24" s="1">
-        <f>[1]Summary!$G27</f>
+        <f ca="1">[1]Summary!$G27</f>
         <v>456</v>
       </c>
       <c r="D24" t="s">
@@ -3546,7 +3546,7 @@
         <v>Certificate</v>
       </c>
       <c r="G24">
-        <f>[1]Summary!$H27</f>
+        <f ca="1">[1]Summary!$H27</f>
         <v>6271</v>
       </c>
       <c r="H24" t="s">
@@ -3578,11 +3578,11 @@
         <v>English As Second Language</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>14.545454545454545</v>
       </c>
       <c r="C25" s="1">
-        <f>[1]Summary!$G28</f>
+        <f ca="1">[1]Summary!$G28</f>
         <v>320</v>
       </c>
       <c r="D25" t="s">
@@ -3596,7 +3596,7 @@
         <v>Certificate</v>
       </c>
       <c r="G25">
-        <f>[1]Summary!$H28</f>
+        <f ca="1">[1]Summary!$H28</f>
         <v>3390</v>
       </c>
       <c r="H25" t="s">
@@ -3628,11 +3628,11 @@
         <v>Entrepreneurial Business Applications Diploma</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>41.18181818181818</v>
       </c>
       <c r="C26" s="1">
-        <f>[1]Summary!$G29</f>
+        <f ca="1">[1]Summary!$G29</f>
         <v>906</v>
       </c>
       <c r="D26" t="s">
@@ -3646,7 +3646,7 @@
         <v>Diploma</v>
       </c>
       <c r="G26">
-        <f>[1]Summary!$H29</f>
+        <f ca="1">[1]Summary!$H29</f>
         <v>12541</v>
       </c>
       <c r="H26" t="s">
@@ -3678,11 +3678,11 @@
         <v>Executive Assistant Diploma</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>48.136363636363633</v>
       </c>
       <c r="C27" s="1">
-        <f>[1]Summary!$G30</f>
+        <f ca="1">[1]Summary!$G30</f>
         <v>1059</v>
       </c>
       <c r="D27" t="s">
@@ -3696,7 +3696,7 @@
         <v>Diploma</v>
       </c>
       <c r="G27">
-        <f>[1]Summary!$H30</f>
+        <f ca="1">[1]Summary!$H30</f>
         <v>14334</v>
       </c>
       <c r="H27" t="s">
@@ -3728,11 +3728,11 @@
         <v>Graphic Designer Diploma</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>49.454545454545453</v>
       </c>
       <c r="C28" s="1">
-        <f>[1]Summary!$G31</f>
+        <f ca="1">[1]Summary!$G31</f>
         <v>1088</v>
       </c>
       <c r="D28" t="s">
@@ -3746,7 +3746,7 @@
         <v>Diploma</v>
       </c>
       <c r="G28">
-        <f>[1]Summary!$H31</f>
+        <f ca="1">[1]Summary!$H31</f>
         <v>16396</v>
       </c>
       <c r="H28" t="s">
@@ -3778,11 +3778,11 @@
         <v>Human Resources Administration Certificate</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>29.09090909090909</v>
       </c>
       <c r="C29" s="1">
-        <f>[1]Summary!$G32</f>
+        <f ca="1">[1]Summary!$G32</f>
         <v>640</v>
       </c>
       <c r="D29" t="s">
@@ -3796,7 +3796,7 @@
         <v>Certificate</v>
       </c>
       <c r="G29">
-        <f>[1]Summary!$H32</f>
+        <f ca="1">[1]Summary!$H32</f>
         <v>8468</v>
       </c>
       <c r="H29" t="s">
@@ -3828,11 +3828,11 @@
         <v>Marketing Administrative Assistant Certificate</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>34.545454545454547</v>
       </c>
       <c r="C30" s="1">
-        <f>[1]Summary!$G33</f>
+        <f ca="1">[1]Summary!$G33</f>
         <v>760</v>
       </c>
       <c r="D30" t="s">
@@ -3846,7 +3846,7 @@
         <v>Certificate</v>
       </c>
       <c r="G30">
-        <f>[1]Summary!$H33</f>
+        <f ca="1">[1]Summary!$H33</f>
         <v>10655</v>
       </c>
       <c r="H30" t="s">
@@ -3878,11 +3878,11 @@
         <v>Marketing Coordinator Diploma</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>43.045454545454547</v>
       </c>
       <c r="C31" s="1">
-        <f>[1]Summary!$G34</f>
+        <f ca="1">[1]Summary!$G34</f>
         <v>947</v>
       </c>
       <c r="D31" t="s">
@@ -3896,7 +3896,7 @@
         <v>Diploma</v>
       </c>
       <c r="G31">
-        <f>[1]Summary!$H34</f>
+        <f ca="1">[1]Summary!$H34</f>
         <v>14242</v>
       </c>
       <c r="H31" t="s">
@@ -3928,11 +3928,11 @@
         <v>Medical Administrative Assistant Certificate</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>39.727272727272727</v>
       </c>
       <c r="C32" s="1">
-        <f>[1]Summary!$G35</f>
+        <f ca="1">[1]Summary!$G35</f>
         <v>874</v>
       </c>
       <c r="D32" t="s">
@@ -3946,7 +3946,7 @@
         <v>Certificate</v>
       </c>
       <c r="G32">
-        <f>[1]Summary!$H35</f>
+        <f ca="1">[1]Summary!$H35</f>
         <v>10875</v>
       </c>
       <c r="H32" t="s">
@@ -3978,11 +3978,11 @@
         <v>Medical Office Assistant Diploma</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ca="1" si="0"/>
         <v>45.81818181818182</v>
       </c>
       <c r="C33" s="1">
-        <f>[1]Summary!$G36</f>
+        <f ca="1">[1]Summary!$G36</f>
         <v>1008</v>
       </c>
       <c r="D33" t="s">
@@ -3996,7 +3996,7 @@
         <v>Diploma</v>
       </c>
       <c r="G33">
-        <f>[1]Summary!$H36</f>
+        <f ca="1">[1]Summary!$H36</f>
         <v>14133</v>
       </c>
       <c r="H33" t="s">
@@ -4028,11 +4028,11 @@
         <v>Medical Office Assistant Diploma W/ Unit Clerk</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" ref="B34:B52" si="5">C34/weeks</f>
+        <f t="shared" ref="B34:B52" ca="1" si="5">C34/weeks</f>
         <v>59.18181818181818</v>
       </c>
       <c r="C34" s="1">
-        <f>[1]Summary!$G37</f>
+        <f ca="1">[1]Summary!$G37</f>
         <v>1302</v>
       </c>
       <c r="D34" t="s">
@@ -4046,7 +4046,7 @@
         <v>Diploma</v>
       </c>
       <c r="G34">
-        <f>[1]Summary!$H37</f>
+        <f ca="1">[1]Summary!$H37</f>
         <v>16455</v>
       </c>
       <c r="H34" t="s">
@@ -4078,11 +4078,11 @@
         <v>Medical Office Front Desk Assistant Certificate</v>
       </c>
       <c r="B35" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>26.09090909090909</v>
       </c>
       <c r="C35" s="1">
-        <f>[1]Summary!$G38</f>
+        <f ca="1">[1]Summary!$G38</f>
         <v>574</v>
       </c>
       <c r="D35" t="s">
@@ -4096,7 +4096,7 @@
         <v>Certificate</v>
       </c>
       <c r="G35">
-        <f>[1]Summary!$H38</f>
+        <f ca="1">[1]Summary!$H38</f>
         <v>7048</v>
       </c>
       <c r="H35" t="s">
@@ -4128,11 +4128,11 @@
         <v>Microsoft Certified Solutions Associate: Server Cert.</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>18.954545454545453</v>
       </c>
       <c r="C36" s="1">
-        <f>[1]Summary!$G39</f>
+        <f ca="1">[1]Summary!$G39</f>
         <v>417</v>
       </c>
       <c r="D36" t="s">
@@ -4146,7 +4146,7 @@
         <v>Certificate</v>
       </c>
       <c r="G36">
-        <f>[1]Summary!$H39</f>
+        <f ca="1">[1]Summary!$H39</f>
         <v>5624</v>
       </c>
       <c r="H36" t="s">
@@ -4178,11 +4178,11 @@
         <v>Microsoft Certified Solutions Associate: Windows</v>
       </c>
       <c r="B37" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>18.954545454545453</v>
       </c>
       <c r="C37" s="1">
-        <f>[1]Summary!$G40</f>
+        <f ca="1">[1]Summary!$G40</f>
         <v>417</v>
       </c>
       <c r="D37" t="s">
@@ -4196,7 +4196,7 @@
         <v>Certificate</v>
       </c>
       <c r="G37">
-        <f>[1]Summary!$H40</f>
+        <f ca="1">[1]Summary!$H40</f>
         <v>5624</v>
       </c>
       <c r="H37" t="s">
@@ -4228,11 +4228,11 @@
         <v>Network Administrator Diploma (Server 2016)</v>
       </c>
       <c r="B38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>79.681818181818187</v>
       </c>
       <c r="C38" s="1">
-        <f>[1]Summary!$G41</f>
+        <f ca="1">[1]Summary!$G41</f>
         <v>1753</v>
       </c>
       <c r="D38" t="s">
@@ -4246,7 +4246,7 @@
         <v>Diploma</v>
       </c>
       <c r="G38">
-        <f>[1]Summary!$H41</f>
+        <f ca="1">[1]Summary!$H41</f>
         <v>20916</v>
       </c>
       <c r="H38" t="s">
@@ -4278,11 +4278,11 @@
         <v>Office Administration Assistant Certificate</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>21.454545454545453</v>
       </c>
       <c r="C39" s="1">
-        <f>[1]Summary!$G42</f>
+        <f ca="1">[1]Summary!$G42</f>
         <v>472</v>
       </c>
       <c r="D39" t="s">
@@ -4296,7 +4296,7 @@
         <v>Certificate</v>
       </c>
       <c r="G39">
-        <f>[1]Summary!$H42</f>
+        <f ca="1">[1]Summary!$H42</f>
         <v>6296</v>
       </c>
       <c r="H39" t="s">
@@ -4328,11 +4328,11 @@
         <v>Office Administration Diploma</v>
       </c>
       <c r="B40" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>48.227272727272727</v>
       </c>
       <c r="C40" s="1">
-        <f>[1]Summary!$G43</f>
+        <f ca="1">[1]Summary!$G43</f>
         <v>1061</v>
       </c>
       <c r="D40" t="s">
@@ -4346,7 +4346,7 @@
         <v>Diploma</v>
       </c>
       <c r="G40">
-        <f>[1]Summary!$H43</f>
+        <f ca="1">[1]Summary!$H43</f>
         <v>14251</v>
       </c>
       <c r="H40" t="s">
@@ -4378,11 +4378,11 @@
         <v>Office Clerk Certificate</v>
       </c>
       <c r="B41" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>19.772727272727273</v>
       </c>
       <c r="C41" s="1">
-        <f>[1]Summary!$G44</f>
+        <f ca="1">[1]Summary!$G44</f>
         <v>435</v>
       </c>
       <c r="D41" t="s">
@@ -4396,7 +4396,7 @@
         <v>Certificate</v>
       </c>
       <c r="G41">
-        <f>[1]Summary!$H44</f>
+        <f ca="1">[1]Summary!$H44</f>
         <v>5487</v>
       </c>
       <c r="H41" t="s">
@@ -4428,11 +4428,11 @@
         <v>Payroll Administrator Certificate</v>
       </c>
       <c r="B42" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>34.227272727272727</v>
       </c>
       <c r="C42" s="1">
-        <f>[1]Summary!$G45</f>
+        <f ca="1">[1]Summary!$G45</f>
         <v>753</v>
       </c>
       <c r="D42" t="s">
@@ -4446,7 +4446,7 @@
         <v>Certificate</v>
       </c>
       <c r="G42">
-        <f>[1]Summary!$H45</f>
+        <f ca="1">[1]Summary!$H45</f>
         <v>10882</v>
       </c>
       <c r="H42" t="s">
@@ -4478,11 +4478,11 @@
         <v>Payroll Clerk Certificate</v>
       </c>
       <c r="B43" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>24.454545454545453</v>
       </c>
       <c r="C43" s="1">
-        <f>[1]Summary!$G46</f>
+        <f ca="1">[1]Summary!$G46</f>
         <v>538</v>
       </c>
       <c r="D43" t="s">
@@ -4496,7 +4496,7 @@
         <v>Certificate</v>
       </c>
       <c r="G43">
-        <f>[1]Summary!$H46</f>
+        <f ca="1">[1]Summary!$H46</f>
         <v>7656</v>
       </c>
       <c r="H43" t="s">
@@ -4528,11 +4528,11 @@
         <v>Pc Support Specialist Diploma</v>
       </c>
       <c r="B44" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>52.909090909090907</v>
       </c>
       <c r="C44" s="1">
-        <f>[1]Summary!$G47</f>
+        <f ca="1">[1]Summary!$G47</f>
         <v>1164</v>
       </c>
       <c r="D44" t="s">
@@ -4546,7 +4546,7 @@
         <v>Diploma</v>
       </c>
       <c r="G44">
-        <f>[1]Summary!$H47</f>
+        <f ca="1">[1]Summary!$H47</f>
         <v>13604</v>
       </c>
       <c r="H44" t="s">
@@ -4578,11 +4578,11 @@
         <v>Project Administration Diploma</v>
       </c>
       <c r="B45" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>45.545454545454547</v>
       </c>
       <c r="C45" s="1">
-        <f>[1]Summary!$G48</f>
+        <f ca="1">[1]Summary!$G48</f>
         <v>1002</v>
       </c>
       <c r="D45" t="s">
@@ -4596,7 +4596,7 @@
         <v>Diploma</v>
       </c>
       <c r="G45">
-        <f>[1]Summary!$H48</f>
+        <f ca="1">[1]Summary!$H48</f>
         <v>14175</v>
       </c>
       <c r="H45" t="s">
@@ -4628,11 +4628,11 @@
         <v>Psa - Computerized Office Skills Certificate</v>
       </c>
       <c r="B46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>10.545454545454545</v>
       </c>
       <c r="C46" s="1">
-        <f>[1]Summary!$G49</f>
+        <f ca="1">[1]Summary!$G49</f>
         <v>232</v>
       </c>
       <c r="D46" t="s">
@@ -4646,7 +4646,7 @@
         <v>Certificate</v>
       </c>
       <c r="G46">
-        <f>[1]Summary!$H49</f>
+        <f ca="1">[1]Summary!$H49</f>
         <v>3471</v>
       </c>
       <c r="H46" t="s">
@@ -4678,11 +4678,11 @@
         <v>Sales Associate Certificate</v>
       </c>
       <c r="B47" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>18.363636363636363</v>
       </c>
       <c r="C47" s="1">
-        <f>[1]Summary!$G50</f>
+        <f ca="1">[1]Summary!$G50</f>
         <v>404</v>
       </c>
       <c r="D47" t="s">
@@ -4696,7 +4696,7 @@
         <v>Certificate</v>
       </c>
       <c r="G47">
-        <f>[1]Summary!$H50</f>
+        <f ca="1">[1]Summary!$H50</f>
         <v>5651</v>
       </c>
       <c r="H47" t="s">
@@ -4728,11 +4728,11 @@
         <v>Sales Professional Diploma</v>
       </c>
       <c r="B48" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>38.363636363636367</v>
       </c>
       <c r="C48" s="1">
-        <f>[1]Summary!$G51</f>
+        <f ca="1">[1]Summary!$G51</f>
         <v>844</v>
       </c>
       <c r="D48" t="s">
@@ -4746,7 +4746,7 @@
         <v>Diploma</v>
       </c>
       <c r="G48">
-        <f>[1]Summary!$H51</f>
+        <f ca="1">[1]Summary!$H51</f>
         <v>11787</v>
       </c>
       <c r="H48" t="s">
@@ -4778,11 +4778,11 @@
         <v>Software And Web Developer Diploma</v>
       </c>
       <c r="B49" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>43.136363636363633</v>
       </c>
       <c r="C49" s="1">
-        <f>[1]Summary!$G52</f>
+        <f ca="1">[1]Summary!$G52</f>
         <v>949</v>
       </c>
       <c r="D49" t="s">
@@ -4796,7 +4796,7 @@
         <v>Diploma</v>
       </c>
       <c r="G49">
-        <f>[1]Summary!$H52</f>
+        <f ca="1">[1]Summary!$H52</f>
         <v>17063</v>
       </c>
       <c r="H49" t="s">
@@ -4828,11 +4828,11 @@
         <v>Web Designer Diploma</v>
       </c>
       <c r="B50" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>53.772727272727273</v>
       </c>
       <c r="C50" s="1">
-        <f>[1]Summary!$G53</f>
+        <f ca="1">[1]Summary!$G53</f>
         <v>1183</v>
       </c>
       <c r="D50" t="s">
@@ -4846,7 +4846,7 @@
         <v>Diploma</v>
       </c>
       <c r="G50">
-        <f>[1]Summary!$H53</f>
+        <f ca="1">[1]Summary!$H53</f>
         <v>17114</v>
       </c>
       <c r="H50" t="s">
@@ -4878,11 +4878,11 @@
         <v>Web Developer Diploma</v>
       </c>
       <c r="B51" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" ca="1" si="5"/>
         <v>26.863636363636363</v>
       </c>
       <c r="C51" s="1">
-        <f>[1]Summary!$G54</f>
+        <f ca="1">[1]Summary!$G54</f>
         <v>591</v>
       </c>
       <c r="D51" t="s">
@@ -4896,7 +4896,7 @@
         <v>Diploma</v>
       </c>
       <c r="G51">
-        <f>[1]Summary!$H54</f>
+        <f ca="1">[1]Summary!$H54</f>
         <v>10774</v>
       </c>
       <c r="H51" t="s">

</xml_diff>